<commit_message>
DMT class - v1.1
</commit_message>
<xml_diff>
--- a/tmp/cervejas.xlsx
+++ b/tmp/cervejas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">Skol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lixol</t>
   </si>
 </sst>
 </file>
@@ -304,10 +307,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -316,7 +319,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -339,7 +342,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -362,7 +365,7 @@
       <c r="F2" s="4" t="n">
         <v>18.9</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -385,7 +388,7 @@
       <c r="F3" s="4" t="n">
         <v>19.8</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -408,7 +411,7 @@
       <c r="F4" s="4" t="n">
         <v>265</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -431,7 +434,7 @@
       <c r="F5" s="4" t="n">
         <v>2.95</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -454,7 +457,7 @@
       <c r="F6" s="4" t="n">
         <v>29.67</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -477,7 +480,7 @@
       <c r="F7" s="4" t="n">
         <v>4.9</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -500,7 +503,7 @@
       <c r="F8" s="4" t="n">
         <v>29.9</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -523,7 +526,7 @@
       <c r="F9" s="4" t="n">
         <v>270</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -546,7 +549,7 @@
       <c r="F10" s="4" t="n">
         <v>32.9</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -569,7 +572,7 @@
       <c r="F11" s="4" t="n">
         <v>21.9</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -592,7 +595,7 @@
       <c r="F12" s="4" t="n">
         <v>19.9</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -615,7 +618,30 @@
       <c r="F13" s="4" t="n">
         <v>2.99</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="2" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="2" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>